<commit_message>
20200228 and 20200301 commit
</commit_message>
<xml_diff>
--- a/病毒走势.xlsx
+++ b/病毒走势.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="55">
   <si>
     <t>全国确诊</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -186,6 +186,21 @@
   <si>
     <t>2月27日</t>
   </si>
+  <si>
+    <t>2月28日</t>
+  </si>
+  <si>
+    <t>3月1日</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>3月1日2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>3月1日</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -263,7 +278,15 @@
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="着色 1" xfId="1" builtinId="29"/>
   </cellStyles>
-  <dxfs count="84">
+  <dxfs count="88">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -553,6 +576,14 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -705,9 +736,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$2:$AN$2</c:f>
+              <c:f>Sheet1!$B$2:$AP$2</c:f>
               <c:strCache>
-                <c:ptCount val="39"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>1月20日</c:v>
                 </c:pt>
@@ -824,16 +855,22 @@
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>2月27日</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2月28日</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3月1日</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$AN$3</c:f>
+              <c:f>Sheet1!$B$3:$AP$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="39"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="1">
                   <c:v>26</c:v>
                 </c:pt>
@@ -947,6 +984,12 @@
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>452</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>248</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>132</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -992,9 +1035,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$2:$AN$2</c:f>
+              <c:f>Sheet1!$B$2:$AP$2</c:f>
               <c:strCache>
-                <c:ptCount val="39"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>1月20日</c:v>
                 </c:pt>
@@ -1111,16 +1154,22 @@
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>2月27日</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2月28日</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3月1日</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$AN$4</c:f>
+              <c:f>Sheet1!$B$4:$AP$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="39"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>77</c:v>
                 </c:pt>
@@ -1237,6 +1286,12 @@
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>327</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>427</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>573</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1282,9 +1337,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$2:$AN$2</c:f>
+              <c:f>Sheet1!$B$2:$AP$2</c:f>
               <c:strCache>
-                <c:ptCount val="39"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>1月20日</c:v>
                 </c:pt>
@@ -1401,16 +1456,22 @@
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>2月27日</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2月28日</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3月1日</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$AN$5</c:f>
+              <c:f>Sheet1!$B$5:$AP$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="39"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="5">
                   <c:v>87</c:v>
                 </c:pt>
@@ -1512,6 +1573,12 @@
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>-394</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-288</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-299</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1580,12 +1647,12 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$B$2:$AN$2</c15:sqref>
+                          <c15:sqref>Sheet1!$B$2:$AP$2</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:strCache>
-                      <c:ptCount val="39"/>
+                      <c:ptCount val="41"/>
                       <c:pt idx="0">
                         <c:v>1月20日</c:v>
                       </c:pt>
@@ -1702,6 +1769,12 @@
                       </c:pt>
                       <c:pt idx="38">
                         <c:v>2月27日</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>2月28日</c:v>
+                      </c:pt>
+                      <c:pt idx="40">
+                        <c:v>3月1日</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -1711,13 +1784,13 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$B$6:$AN$6</c15:sqref>
+                          <c15:sqref>Sheet1!$B$6:$AP$6</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="39"/>
+                      <c:ptCount val="41"/>
                       <c:pt idx="1">
                         <c:v>3</c:v>
                       </c:pt>
@@ -1831,6 +1904,12 @@
                       </c:pt>
                       <c:pt idx="38">
                         <c:v>44</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>47</c:v>
+                      </c:pt>
+                      <c:pt idx="40">
+                        <c:v>35</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1887,12 +1966,12 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$B$2:$AN$2</c15:sqref>
+                          <c15:sqref>Sheet1!$B$2:$AP$2</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:strCache>
-                      <c:ptCount val="39"/>
+                      <c:ptCount val="41"/>
                       <c:pt idx="0">
                         <c:v>1月20日</c:v>
                       </c:pt>
@@ -2009,6 +2088,12 @@
                       </c:pt>
                       <c:pt idx="38">
                         <c:v>2月27日</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>2月28日</c:v>
+                      </c:pt>
+                      <c:pt idx="40">
+                        <c:v>3月1日</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -2018,13 +2103,13 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$B$7:$AN$7</c15:sqref>
+                          <c15:sqref>Sheet1!$B$7:$AP$7</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="39"/>
+                      <c:ptCount val="41"/>
                       <c:pt idx="3">
                         <c:v>6</c:v>
                       </c:pt>
@@ -2132,6 +2217,12 @@
                       </c:pt>
                       <c:pt idx="38">
                         <c:v>3622</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>2885</c:v>
+                      </c:pt>
+                      <c:pt idx="40">
+                        <c:v>2623</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2473,9 +2564,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$9:$AN$9</c:f>
+              <c:f>Sheet1!$B$9:$AP$9</c:f>
               <c:strCache>
-                <c:ptCount val="39"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>1月20日</c:v>
                 </c:pt>
@@ -2592,16 +2683,22 @@
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>2月27日</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3月1日</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3月1日2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$10:$AN$10</c:f>
+              <c:f>Sheet1!$B$10:$AP$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="39"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>54</c:v>
                 </c:pt>
@@ -2718,6 +2815,12 @@
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>2308</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1418</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>851</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2763,9 +2866,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$9:$AN$9</c:f>
+              <c:f>Sheet1!$B$9:$AP$9</c:f>
               <c:strCache>
-                <c:ptCount val="39"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>1月20日</c:v>
                 </c:pt>
@@ -2882,16 +2985,22 @@
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>2月27日</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3月1日</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3月1日2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$11:$AN$11</c:f>
+              <c:f>Sheet1!$B$11:$AP$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="39"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>291</c:v>
                 </c:pt>
@@ -3008,6 +3117,12 @@
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>39919</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>37414</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>35329</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3053,9 +3168,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$9:$AN$9</c:f>
+              <c:f>Sheet1!$B$9:$AP$9</c:f>
               <c:strCache>
-                <c:ptCount val="39"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>1月20日</c:v>
                 </c:pt>
@@ -3172,16 +3287,22 @@
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>2月27日</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3月1日</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3月1日2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$12:$AN$12</c:f>
+              <c:f>Sheet1!$B$12:$AP$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="39"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="1">
                   <c:v>102</c:v>
                 </c:pt>
@@ -3295,6 +3416,12 @@
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>7952</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>7664</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>7365</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3303,6 +3430,298 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-C29E-44F5-A0E4-1C6EF4F32762}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>全国治愈</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:srgbClr val="00B050">
+                  <a:alpha val="14000"/>
+                </a:srgbClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$9:$AP$9</c:f>
+              <c:strCache>
+                <c:ptCount val="41"/>
+                <c:pt idx="0">
+                  <c:v>1月20日</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1月21日</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1月22日</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1月23日</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1月24日</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1月25日</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1月26日</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1月27日</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1月28日</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1月29日</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1月30日</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1月31日</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2月1日</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2月2日</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2月3日</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2月4日</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2月5日</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2月6日</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2月7日</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2月8日</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2月9日</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2月10日</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2月11日</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2月12日</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2月13日</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2月14日</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2月15日</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2月16日</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2月17日</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2月18日</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2月19日</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2月20日</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2月21日</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2月22日</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2月23日</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2月24日</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2月25日</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2月26日</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2月27日</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3月1日</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3月1日2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$14:$AP$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="41"/>
+                <c:pt idx="3">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>171</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>243</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>328</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>475</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>632</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>892</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1153</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1540</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2050</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2649</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3281</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3996</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4740</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5911</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>6723</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8096</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>9419</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>10844</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>12552</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>14376</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>16155</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>18264</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>20659</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>22888</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>24734</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>27323</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>29745</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>32495</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>36117</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>39002</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41625</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F060-404F-A1D2-818F8331EDD7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3363,12 +3782,12 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$B$9:$AN$9</c15:sqref>
+                          <c15:sqref>Sheet1!$B$9:$AP$9</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:strCache>
-                      <c:ptCount val="39"/>
+                      <c:ptCount val="41"/>
                       <c:pt idx="0">
                         <c:v>1月20日</c:v>
                       </c:pt>
@@ -3485,6 +3904,12 @@
                       </c:pt>
                       <c:pt idx="38">
                         <c:v>2月27日</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>3月1日</c:v>
+                      </c:pt>
+                      <c:pt idx="40">
+                        <c:v>3月1日2</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -3494,13 +3919,13 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$B$13:$AN$13</c15:sqref>
+                          <c15:sqref>Sheet1!$B$13:$AP$13</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="39"/>
+                      <c:ptCount val="41"/>
                       <c:pt idx="1">
                         <c:v>9</c:v>
                       </c:pt>
@@ -3614,6 +4039,12 @@
                       </c:pt>
                       <c:pt idx="38">
                         <c:v>2788</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>2835</c:v>
+                      </c:pt>
+                      <c:pt idx="40">
+                        <c:v>2870</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3622,306 +4053,6 @@
                 <c:extLst>
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000000-9C02-464B-AA9B-1AE93F714B77}"/>
-                  </c:ext>
-                </c:extLst>
-              </c15:ser>
-            </c15:filteredLineSeries>
-            <c15:filteredLineSeries>
-              <c15:ser>
-                <c:idx val="4"/>
-                <c:order val="4"/>
-                <c:tx>
-                  <c:strRef>
-                    <c:extLst>
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$A$14</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:strCache>
-                      <c:ptCount val="1"/>
-                      <c:pt idx="0">
-                        <c:v>全国治愈</c:v>
-                      </c:pt>
-                    </c:strCache>
-                  </c:strRef>
-                </c:tx>
-                <c:spPr>
-                  <a:ln w="22225" cap="rnd">
-                    <a:solidFill>
-                      <a:srgbClr val="00B050"/>
-                    </a:solidFill>
-                  </a:ln>
-                  <a:effectLst>
-                    <a:glow rad="139700">
-                      <a:srgbClr val="00B050">
-                        <a:alpha val="14000"/>
-                      </a:srgbClr>
-                    </a:glow>
-                  </a:effectLst>
-                </c:spPr>
-                <c:marker>
-                  <c:symbol val="none"/>
-                </c:marker>
-                <c:cat>
-                  <c:strRef>
-                    <c:extLst>
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$B$9:$AN$9</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:strCache>
-                      <c:ptCount val="39"/>
-                      <c:pt idx="0">
-                        <c:v>1月20日</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>1月21日</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>1月22日</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>1月23日</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>1月24日</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>1月25日</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>1月26日</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>1月27日</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>1月28日</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>1月29日</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>1月30日</c:v>
-                      </c:pt>
-                      <c:pt idx="11">
-                        <c:v>1月31日</c:v>
-                      </c:pt>
-                      <c:pt idx="12">
-                        <c:v>2月1日</c:v>
-                      </c:pt>
-                      <c:pt idx="13">
-                        <c:v>2月2日</c:v>
-                      </c:pt>
-                      <c:pt idx="14">
-                        <c:v>2月3日</c:v>
-                      </c:pt>
-                      <c:pt idx="15">
-                        <c:v>2月4日</c:v>
-                      </c:pt>
-                      <c:pt idx="16">
-                        <c:v>2月5日</c:v>
-                      </c:pt>
-                      <c:pt idx="17">
-                        <c:v>2月6日</c:v>
-                      </c:pt>
-                      <c:pt idx="18">
-                        <c:v>2月7日</c:v>
-                      </c:pt>
-                      <c:pt idx="19">
-                        <c:v>2月8日</c:v>
-                      </c:pt>
-                      <c:pt idx="20">
-                        <c:v>2月9日</c:v>
-                      </c:pt>
-                      <c:pt idx="21">
-                        <c:v>2月10日</c:v>
-                      </c:pt>
-                      <c:pt idx="22">
-                        <c:v>2月11日</c:v>
-                      </c:pt>
-                      <c:pt idx="23">
-                        <c:v>2月12日</c:v>
-                      </c:pt>
-                      <c:pt idx="24">
-                        <c:v>2月13日</c:v>
-                      </c:pt>
-                      <c:pt idx="25">
-                        <c:v>2月14日</c:v>
-                      </c:pt>
-                      <c:pt idx="26">
-                        <c:v>2月15日</c:v>
-                      </c:pt>
-                      <c:pt idx="27">
-                        <c:v>2月16日</c:v>
-                      </c:pt>
-                      <c:pt idx="28">
-                        <c:v>2月17日</c:v>
-                      </c:pt>
-                      <c:pt idx="29">
-                        <c:v>2月18日</c:v>
-                      </c:pt>
-                      <c:pt idx="30">
-                        <c:v>2月19日</c:v>
-                      </c:pt>
-                      <c:pt idx="31">
-                        <c:v>2月20日</c:v>
-                      </c:pt>
-                      <c:pt idx="32">
-                        <c:v>2月21日</c:v>
-                      </c:pt>
-                      <c:pt idx="33">
-                        <c:v>2月22日</c:v>
-                      </c:pt>
-                      <c:pt idx="34">
-                        <c:v>2月23日</c:v>
-                      </c:pt>
-                      <c:pt idx="35">
-                        <c:v>2月24日</c:v>
-                      </c:pt>
-                      <c:pt idx="36">
-                        <c:v>2月25日</c:v>
-                      </c:pt>
-                      <c:pt idx="37">
-                        <c:v>2月26日</c:v>
-                      </c:pt>
-                      <c:pt idx="38">
-                        <c:v>2月27日</c:v>
-                      </c:pt>
-                    </c:strCache>
-                  </c:strRef>
-                </c:cat>
-                <c:val>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$B$14:$AN$14</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="39"/>
-                      <c:pt idx="3">
-                        <c:v>34</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>38</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>49</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>51</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>60</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>103</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>124</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>171</c:v>
-                      </c:pt>
-                      <c:pt idx="11">
-                        <c:v>243</c:v>
-                      </c:pt>
-                      <c:pt idx="12">
-                        <c:v>328</c:v>
-                      </c:pt>
-                      <c:pt idx="13">
-                        <c:v>475</c:v>
-                      </c:pt>
-                      <c:pt idx="14">
-                        <c:v>632</c:v>
-                      </c:pt>
-                      <c:pt idx="15">
-                        <c:v>892</c:v>
-                      </c:pt>
-                      <c:pt idx="16">
-                        <c:v>1153</c:v>
-                      </c:pt>
-                      <c:pt idx="17">
-                        <c:v>1540</c:v>
-                      </c:pt>
-                      <c:pt idx="18">
-                        <c:v>2050</c:v>
-                      </c:pt>
-                      <c:pt idx="19">
-                        <c:v>2649</c:v>
-                      </c:pt>
-                      <c:pt idx="20">
-                        <c:v>3281</c:v>
-                      </c:pt>
-                      <c:pt idx="21">
-                        <c:v>3996</c:v>
-                      </c:pt>
-                      <c:pt idx="22">
-                        <c:v>4740</c:v>
-                      </c:pt>
-                      <c:pt idx="23">
-                        <c:v>5911</c:v>
-                      </c:pt>
-                      <c:pt idx="24">
-                        <c:v>6723</c:v>
-                      </c:pt>
-                      <c:pt idx="25">
-                        <c:v>8096</c:v>
-                      </c:pt>
-                      <c:pt idx="26">
-                        <c:v>9419</c:v>
-                      </c:pt>
-                      <c:pt idx="27">
-                        <c:v>10844</c:v>
-                      </c:pt>
-                      <c:pt idx="28">
-                        <c:v>12552</c:v>
-                      </c:pt>
-                      <c:pt idx="29">
-                        <c:v>14376</c:v>
-                      </c:pt>
-                      <c:pt idx="30">
-                        <c:v>16155</c:v>
-                      </c:pt>
-                      <c:pt idx="31">
-                        <c:v>18264</c:v>
-                      </c:pt>
-                      <c:pt idx="32">
-                        <c:v>20659</c:v>
-                      </c:pt>
-                      <c:pt idx="33">
-                        <c:v>22888</c:v>
-                      </c:pt>
-                      <c:pt idx="34">
-                        <c:v>24734</c:v>
-                      </c:pt>
-                      <c:pt idx="35">
-                        <c:v>27323</c:v>
-                      </c:pt>
-                      <c:pt idx="36">
-                        <c:v>29745</c:v>
-                      </c:pt>
-                      <c:pt idx="37">
-                        <c:v>32495</c:v>
-                      </c:pt>
-                      <c:pt idx="38">
-                        <c:v>36117</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:val>
-                <c:smooth val="0"/>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000000-F060-404F-A1D2-818F8331EDD7}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
@@ -4255,9 +4386,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$9:$AN$9</c:f>
+              <c:f>Sheet1!$B$9:$AO$9</c:f>
               <c:strCache>
-                <c:ptCount val="39"/>
+                <c:ptCount val="40"/>
                 <c:pt idx="0">
                   <c:v>1月20日</c:v>
                 </c:pt>
@@ -4374,16 +4505,19 @@
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>2月27日</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3月1日</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$13:$AN$13</c:f>
+              <c:f>Sheet1!$B$13:$AO$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="39"/>
+                <c:ptCount val="40"/>
                 <c:pt idx="1">
                   <c:v>9</c:v>
                 </c:pt>
@@ -4497,6 +4631,9 @@
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>2788</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2835</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4541,9 +4678,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$9:$AN$9</c:f>
+              <c:f>Sheet1!$B$9:$AO$9</c:f>
               <c:strCache>
-                <c:ptCount val="39"/>
+                <c:ptCount val="40"/>
                 <c:pt idx="0">
                   <c:v>1月20日</c:v>
                 </c:pt>
@@ -4660,16 +4797,19 @@
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>2月27日</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3月1日</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$14:$AN$14</c:f>
+              <c:f>Sheet1!$B$14:$AO$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="39"/>
+                <c:ptCount val="40"/>
                 <c:pt idx="3">
                   <c:v>34</c:v>
                 </c:pt>
@@ -4777,6 +4917,9 @@
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>36117</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>39002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4845,12 +4988,12 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$B$9:$AN$9</c15:sqref>
+                          <c15:sqref>Sheet1!$B$9:$AO$9</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:strCache>
-                      <c:ptCount val="39"/>
+                      <c:ptCount val="40"/>
                       <c:pt idx="0">
                         <c:v>1月20日</c:v>
                       </c:pt>
@@ -4967,6 +5110,9 @@
                       </c:pt>
                       <c:pt idx="38">
                         <c:v>2月27日</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>3月1日</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -4976,13 +5122,13 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$B$10:$AN$10</c15:sqref>
+                          <c15:sqref>Sheet1!$B$10:$AO$10</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="39"/>
+                      <c:ptCount val="40"/>
                       <c:pt idx="0">
                         <c:v>54</c:v>
                       </c:pt>
@@ -5099,6 +5245,9 @@
                       </c:pt>
                       <c:pt idx="38">
                         <c:v>2308</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>1418</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -5117,7 +5266,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$A$11</c15:sqref>
@@ -5152,15 +5301,15 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$B$9:$AN$9</c15:sqref>
+                          <c15:sqref>Sheet1!$B$9:$AO$9</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:strCache>
-                      <c:ptCount val="39"/>
+                      <c:ptCount val="40"/>
                       <c:pt idx="0">
                         <c:v>1月20日</c:v>
                       </c:pt>
@@ -5277,22 +5426,25 @@
                       </c:pt>
                       <c:pt idx="38">
                         <c:v>2月27日</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>3月1日</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$B$11:$AN$11</c15:sqref>
+                          <c15:sqref>Sheet1!$B$11:$AO$11</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="39"/>
+                      <c:ptCount val="40"/>
                       <c:pt idx="0">
                         <c:v>291</c:v>
                       </c:pt>
@@ -5409,6 +5561,9 @@
                       </c:pt>
                       <c:pt idx="38">
                         <c:v>39919</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>37414</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -5427,7 +5582,7 @@
                 <c:order val="2"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$A$12</c15:sqref>
@@ -5462,15 +5617,15 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$B$9:$AN$9</c15:sqref>
+                          <c15:sqref>Sheet1!$B$9:$AO$9</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:strCache>
-                      <c:ptCount val="39"/>
+                      <c:ptCount val="40"/>
                       <c:pt idx="0">
                         <c:v>1月20日</c:v>
                       </c:pt>
@@ -5587,22 +5742,25 @@
                       </c:pt>
                       <c:pt idx="38">
                         <c:v>2月27日</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>3月1日</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$B$12:$AN$12</c15:sqref>
+                          <c15:sqref>Sheet1!$B$12:$AO$12</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="39"/>
+                      <c:ptCount val="40"/>
                       <c:pt idx="1">
                         <c:v>102</c:v>
                       </c:pt>
@@ -5716,6 +5874,9 @@
                       </c:pt>
                       <c:pt idx="38">
                         <c:v>7952</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>7664</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -6053,9 +6214,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$2:$AN$2</c:f>
+              <c:f>Sheet1!$B$2:$AO$2</c:f>
               <c:strCache>
-                <c:ptCount val="39"/>
+                <c:ptCount val="40"/>
                 <c:pt idx="0">
                   <c:v>1月20日</c:v>
                 </c:pt>
@@ -6172,16 +6333,19 @@
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>2月27日</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2月28日</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$6:$AN$6</c:f>
+              <c:f>Sheet1!$B$6:$AO$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="39"/>
+                <c:ptCount val="40"/>
                 <c:pt idx="1">
                   <c:v>3</c:v>
                 </c:pt>
@@ -6295,6 +6459,9 @@
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>47</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6339,9 +6506,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$2:$AN$2</c:f>
+              <c:f>Sheet1!$B$2:$AO$2</c:f>
               <c:strCache>
-                <c:ptCount val="39"/>
+                <c:ptCount val="40"/>
                 <c:pt idx="0">
                   <c:v>1月20日</c:v>
                 </c:pt>
@@ -6458,16 +6625,19 @@
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>2月27日</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2月28日</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$7:$AN$7</c:f>
+              <c:f>Sheet1!$B$7:$AO$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="39"/>
+                <c:ptCount val="40"/>
                 <c:pt idx="3">
                   <c:v>6</c:v>
                 </c:pt>
@@ -6575,6 +6745,9 @@
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>3622</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2885</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6643,12 +6816,12 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$B$2:$AN$2</c15:sqref>
+                          <c15:sqref>Sheet1!$B$2:$AO$2</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:strCache>
-                      <c:ptCount val="39"/>
+                      <c:ptCount val="40"/>
                       <c:pt idx="0">
                         <c:v>1月20日</c:v>
                       </c:pt>
@@ -6765,6 +6938,9 @@
                       </c:pt>
                       <c:pt idx="38">
                         <c:v>2月27日</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>2月28日</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -6774,13 +6950,13 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$B$3:$AN$3</c15:sqref>
+                          <c15:sqref>Sheet1!$B$3:$AO$3</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="39"/>
+                      <c:ptCount val="40"/>
                       <c:pt idx="1">
                         <c:v>26</c:v>
                       </c:pt>
@@ -6894,6 +7070,9 @@
                       </c:pt>
                       <c:pt idx="38">
                         <c:v>452</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>248</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -6912,7 +7091,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$A$4</c15:sqref>
@@ -6947,15 +7126,15 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$B$2:$AN$2</c15:sqref>
+                          <c15:sqref>Sheet1!$B$2:$AO$2</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:strCache>
-                      <c:ptCount val="39"/>
+                      <c:ptCount val="40"/>
                       <c:pt idx="0">
                         <c:v>1月20日</c:v>
                       </c:pt>
@@ -7072,22 +7251,25 @@
                       </c:pt>
                       <c:pt idx="38">
                         <c:v>2月27日</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>2月28日</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$B$4:$AN$4</c15:sqref>
+                          <c15:sqref>Sheet1!$B$4:$AO$4</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="39"/>
+                      <c:ptCount val="40"/>
                       <c:pt idx="0">
                         <c:v>77</c:v>
                       </c:pt>
@@ -7204,6 +7386,9 @@
                       </c:pt>
                       <c:pt idx="38">
                         <c:v>327</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>427</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -7222,7 +7407,7 @@
                 <c:order val="2"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$A$5</c15:sqref>
@@ -7257,15 +7442,15 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$B$2:$AN$2</c15:sqref>
+                          <c15:sqref>Sheet1!$B$2:$AO$2</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:strCache>
-                      <c:ptCount val="39"/>
+                      <c:ptCount val="40"/>
                       <c:pt idx="0">
                         <c:v>1月20日</c:v>
                       </c:pt>
@@ -7382,22 +7567,25 @@
                       </c:pt>
                       <c:pt idx="38">
                         <c:v>2月27日</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>2月28日</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$B$5:$AN$5</c15:sqref>
+                          <c15:sqref>Sheet1!$B$5:$AO$5</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="39"/>
+                      <c:ptCount val="40"/>
                       <c:pt idx="5">
                         <c:v>87</c:v>
                       </c:pt>
@@ -7499,6 +7687,9 @@
                       </c:pt>
                       <c:pt idx="38">
                         <c:v>-394</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>-288</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -10214,98 +10405,102 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="表5" displayName="表5" ref="A2:AN7" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82" headerRowCellStyle="着色 1">
-  <autoFilter ref="A2:AN7"/>
-  <tableColumns count="40">
-    <tableColumn id="1" name="新增" dataDxfId="81" dataCellStyle="着色 1"/>
-    <tableColumn id="2" name="1月20日" dataDxfId="80"/>
-    <tableColumn id="3" name="1月21日" dataDxfId="79"/>
-    <tableColumn id="4" name="1月22日" dataDxfId="78"/>
-    <tableColumn id="5" name="1月23日" dataDxfId="77"/>
-    <tableColumn id="6" name="1月24日" dataDxfId="76"/>
-    <tableColumn id="7" name="1月25日" dataDxfId="75"/>
-    <tableColumn id="8" name="1月26日" dataDxfId="74"/>
-    <tableColumn id="9" name="1月27日" dataDxfId="73"/>
-    <tableColumn id="10" name="1月28日" dataDxfId="72"/>
-    <tableColumn id="11" name="1月29日" dataDxfId="71"/>
-    <tableColumn id="12" name="1月30日" dataDxfId="70"/>
-    <tableColumn id="13" name="1月31日" dataDxfId="69"/>
-    <tableColumn id="14" name="2月1日" dataDxfId="68"/>
-    <tableColumn id="15" name="2月2日" dataDxfId="67"/>
-    <tableColumn id="16" name="2月3日" dataDxfId="66"/>
-    <tableColumn id="17" name="2月4日" dataDxfId="65"/>
-    <tableColumn id="18" name="2月5日" dataDxfId="64"/>
-    <tableColumn id="19" name="2月6日" dataDxfId="63"/>
-    <tableColumn id="20" name="2月7日" dataDxfId="62"/>
-    <tableColumn id="21" name="2月8日" dataDxfId="61"/>
-    <tableColumn id="22" name="2月9日" dataDxfId="60"/>
-    <tableColumn id="23" name="2月10日" dataDxfId="59"/>
-    <tableColumn id="24" name="2月11日" dataDxfId="58"/>
-    <tableColumn id="25" name="2月12日" dataDxfId="57"/>
-    <tableColumn id="26" name="2月13日" dataDxfId="56"/>
-    <tableColumn id="27" name="2月14日" dataDxfId="55"/>
-    <tableColumn id="28" name="2月15日" dataDxfId="54"/>
-    <tableColumn id="29" name="2月16日" dataDxfId="53"/>
-    <tableColumn id="30" name="2月17日" dataDxfId="52"/>
-    <tableColumn id="31" name="2月18日" dataDxfId="51"/>
-    <tableColumn id="32" name="2月19日" dataDxfId="50"/>
-    <tableColumn id="33" name="2月20日" dataDxfId="49"/>
-    <tableColumn id="34" name="2月21日" dataDxfId="48"/>
-    <tableColumn id="35" name="2月22日" dataDxfId="47"/>
-    <tableColumn id="36" name="2月23日" dataDxfId="46"/>
-    <tableColumn id="37" name="2月24日" dataDxfId="45"/>
-    <tableColumn id="38" name="2月25日" dataDxfId="44"/>
-    <tableColumn id="39" name="2月26日" dataDxfId="43"/>
-    <tableColumn id="40" name="2月27日" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="表5" displayName="表5" ref="A2:AP7" totalsRowShown="0" headerRowDxfId="87" dataDxfId="86" headerRowCellStyle="着色 1">
+  <autoFilter ref="A2:AP7"/>
+  <tableColumns count="42">
+    <tableColumn id="1" name="新增" dataDxfId="85" dataCellStyle="着色 1"/>
+    <tableColumn id="2" name="1月20日" dataDxfId="84"/>
+    <tableColumn id="3" name="1月21日" dataDxfId="83"/>
+    <tableColumn id="4" name="1月22日" dataDxfId="82"/>
+    <tableColumn id="5" name="1月23日" dataDxfId="81"/>
+    <tableColumn id="6" name="1月24日" dataDxfId="80"/>
+    <tableColumn id="7" name="1月25日" dataDxfId="79"/>
+    <tableColumn id="8" name="1月26日" dataDxfId="78"/>
+    <tableColumn id="9" name="1月27日" dataDxfId="77"/>
+    <tableColumn id="10" name="1月28日" dataDxfId="76"/>
+    <tableColumn id="11" name="1月29日" dataDxfId="75"/>
+    <tableColumn id="12" name="1月30日" dataDxfId="74"/>
+    <tableColumn id="13" name="1月31日" dataDxfId="73"/>
+    <tableColumn id="14" name="2月1日" dataDxfId="72"/>
+    <tableColumn id="15" name="2月2日" dataDxfId="71"/>
+    <tableColumn id="16" name="2月3日" dataDxfId="70"/>
+    <tableColumn id="17" name="2月4日" dataDxfId="69"/>
+    <tableColumn id="18" name="2月5日" dataDxfId="68"/>
+    <tableColumn id="19" name="2月6日" dataDxfId="67"/>
+    <tableColumn id="20" name="2月7日" dataDxfId="66"/>
+    <tableColumn id="21" name="2月8日" dataDxfId="65"/>
+    <tableColumn id="22" name="2月9日" dataDxfId="64"/>
+    <tableColumn id="23" name="2月10日" dataDxfId="63"/>
+    <tableColumn id="24" name="2月11日" dataDxfId="62"/>
+    <tableColumn id="25" name="2月12日" dataDxfId="61"/>
+    <tableColumn id="26" name="2月13日" dataDxfId="60"/>
+    <tableColumn id="27" name="2月14日" dataDxfId="59"/>
+    <tableColumn id="28" name="2月15日" dataDxfId="58"/>
+    <tableColumn id="29" name="2月16日" dataDxfId="57"/>
+    <tableColumn id="30" name="2月17日" dataDxfId="56"/>
+    <tableColumn id="31" name="2月18日" dataDxfId="55"/>
+    <tableColumn id="32" name="2月19日" dataDxfId="54"/>
+    <tableColumn id="33" name="2月20日" dataDxfId="53"/>
+    <tableColumn id="34" name="2月21日" dataDxfId="52"/>
+    <tableColumn id="35" name="2月22日" dataDxfId="51"/>
+    <tableColumn id="36" name="2月23日" dataDxfId="50"/>
+    <tableColumn id="37" name="2月24日" dataDxfId="49"/>
+    <tableColumn id="38" name="2月25日" dataDxfId="48"/>
+    <tableColumn id="39" name="2月26日" dataDxfId="47"/>
+    <tableColumn id="40" name="2月27日" dataDxfId="46"/>
+    <tableColumn id="41" name="2月28日" dataDxfId="45"/>
+    <tableColumn id="42" name="3月1日" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="表6" displayName="表6" ref="A9:AN14" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41" headerRowCellStyle="着色 1">
-  <autoFilter ref="A9:AN14"/>
-  <tableColumns count="40">
-    <tableColumn id="1" name="共计" dataDxfId="40" dataCellStyle="着色 1"/>
-    <tableColumn id="2" name="1月20日" dataDxfId="39"/>
-    <tableColumn id="3" name="1月21日" dataDxfId="38"/>
-    <tableColumn id="4" name="1月22日" dataDxfId="37"/>
-    <tableColumn id="5" name="1月23日" dataDxfId="36"/>
-    <tableColumn id="6" name="1月24日" dataDxfId="35"/>
-    <tableColumn id="7" name="1月25日" dataDxfId="34"/>
-    <tableColumn id="8" name="1月26日" dataDxfId="33"/>
-    <tableColumn id="9" name="1月27日" dataDxfId="32"/>
-    <tableColumn id="10" name="1月28日" dataDxfId="31"/>
-    <tableColumn id="11" name="1月29日" dataDxfId="30"/>
-    <tableColumn id="12" name="1月30日" dataDxfId="29"/>
-    <tableColumn id="13" name="1月31日" dataDxfId="28"/>
-    <tableColumn id="14" name="2月1日" dataDxfId="27"/>
-    <tableColumn id="15" name="2月2日" dataDxfId="26"/>
-    <tableColumn id="16" name="2月3日" dataDxfId="25"/>
-    <tableColumn id="17" name="2月4日" dataDxfId="24"/>
-    <tableColumn id="18" name="2月5日" dataDxfId="23"/>
-    <tableColumn id="19" name="2月6日" dataDxfId="22"/>
-    <tableColumn id="20" name="2月7日" dataDxfId="21"/>
-    <tableColumn id="21" name="2月8日" dataDxfId="20"/>
-    <tableColumn id="22" name="2月9日" dataDxfId="19"/>
-    <tableColumn id="23" name="2月10日" dataDxfId="18"/>
-    <tableColumn id="24" name="2月11日" dataDxfId="17"/>
-    <tableColumn id="25" name="2月12日" dataDxfId="16"/>
-    <tableColumn id="26" name="2月13日" dataDxfId="15"/>
-    <tableColumn id="27" name="2月14日" dataDxfId="14"/>
-    <tableColumn id="28" name="2月15日" dataDxfId="13"/>
-    <tableColumn id="29" name="2月16日" dataDxfId="12"/>
-    <tableColumn id="30" name="2月17日" dataDxfId="11"/>
-    <tableColumn id="31" name="2月18日" dataDxfId="10"/>
-    <tableColumn id="32" name="2月19日" dataDxfId="9"/>
-    <tableColumn id="33" name="2月20日" dataDxfId="8"/>
-    <tableColumn id="34" name="2月21日" dataDxfId="7"/>
-    <tableColumn id="35" name="2月22日" dataDxfId="6"/>
-    <tableColumn id="36" name="2月23日" dataDxfId="5"/>
-    <tableColumn id="37" name="2月24日" dataDxfId="4"/>
-    <tableColumn id="38" name="2月25日" dataDxfId="3"/>
-    <tableColumn id="39" name="2月26日" dataDxfId="2"/>
-    <tableColumn id="40" name="2月27日" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="表6" displayName="表6" ref="A9:AP14" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43" headerRowCellStyle="着色 1">
+  <autoFilter ref="A9:AP14"/>
+  <tableColumns count="42">
+    <tableColumn id="1" name="共计" dataDxfId="42" dataCellStyle="着色 1"/>
+    <tableColumn id="2" name="1月20日" dataDxfId="41"/>
+    <tableColumn id="3" name="1月21日" dataDxfId="40"/>
+    <tableColumn id="4" name="1月22日" dataDxfId="39"/>
+    <tableColumn id="5" name="1月23日" dataDxfId="38"/>
+    <tableColumn id="6" name="1月24日" dataDxfId="37"/>
+    <tableColumn id="7" name="1月25日" dataDxfId="36"/>
+    <tableColumn id="8" name="1月26日" dataDxfId="35"/>
+    <tableColumn id="9" name="1月27日" dataDxfId="34"/>
+    <tableColumn id="10" name="1月28日" dataDxfId="33"/>
+    <tableColumn id="11" name="1月29日" dataDxfId="32"/>
+    <tableColumn id="12" name="1月30日" dataDxfId="31"/>
+    <tableColumn id="13" name="1月31日" dataDxfId="30"/>
+    <tableColumn id="14" name="2月1日" dataDxfId="29"/>
+    <tableColumn id="15" name="2月2日" dataDxfId="28"/>
+    <tableColumn id="16" name="2月3日" dataDxfId="27"/>
+    <tableColumn id="17" name="2月4日" dataDxfId="26"/>
+    <tableColumn id="18" name="2月5日" dataDxfId="25"/>
+    <tableColumn id="19" name="2月6日" dataDxfId="24"/>
+    <tableColumn id="20" name="2月7日" dataDxfId="23"/>
+    <tableColumn id="21" name="2月8日" dataDxfId="22"/>
+    <tableColumn id="22" name="2月9日" dataDxfId="21"/>
+    <tableColumn id="23" name="2月10日" dataDxfId="20"/>
+    <tableColumn id="24" name="2月11日" dataDxfId="19"/>
+    <tableColumn id="25" name="2月12日" dataDxfId="18"/>
+    <tableColumn id="26" name="2月13日" dataDxfId="17"/>
+    <tableColumn id="27" name="2月14日" dataDxfId="16"/>
+    <tableColumn id="28" name="2月15日" dataDxfId="15"/>
+    <tableColumn id="29" name="2月16日" dataDxfId="14"/>
+    <tableColumn id="30" name="2月17日" dataDxfId="13"/>
+    <tableColumn id="31" name="2月18日" dataDxfId="12"/>
+    <tableColumn id="32" name="2月19日" dataDxfId="11"/>
+    <tableColumn id="33" name="2月20日" dataDxfId="10"/>
+    <tableColumn id="34" name="2月21日" dataDxfId="9"/>
+    <tableColumn id="35" name="2月22日" dataDxfId="8"/>
+    <tableColumn id="36" name="2月23日" dataDxfId="7"/>
+    <tableColumn id="37" name="2月24日" dataDxfId="6"/>
+    <tableColumn id="38" name="2月25日" dataDxfId="5"/>
+    <tableColumn id="39" name="2月26日" dataDxfId="4"/>
+    <tableColumn id="40" name="2月27日" dataDxfId="3"/>
+    <tableColumn id="41" name="3月1日" dataDxfId="2"/>
+    <tableColumn id="42" name="3月1日2" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -10574,10 +10769,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AN14"/>
+  <dimension ref="A1:AP14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AN14" sqref="AN14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AO29" sqref="AO29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -10587,10 +10782,10 @@
     <col min="31" max="31" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
       <c r="O1" s="2"/>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -10711,8 +10906,14 @@
       <c r="AN2" s="4" t="s">
         <v>50</v>
       </c>
+      <c r="AO2" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AP2" s="4" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>26</v>
       </c>
@@ -10831,8 +11032,14 @@
       <c r="AN3" s="5">
         <v>452</v>
       </c>
+      <c r="AO3" s="5">
+        <v>248</v>
+      </c>
+      <c r="AP3" s="5">
+        <v>132</v>
+      </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -10953,8 +11160,14 @@
       <c r="AN4" s="5">
         <v>327</v>
       </c>
+      <c r="AO4" s="5">
+        <v>427</v>
+      </c>
+      <c r="AP4" s="5">
+        <v>573</v>
+      </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
@@ -11065,8 +11278,14 @@
       <c r="AN5" s="5">
         <v>-394</v>
       </c>
+      <c r="AO5" s="5">
+        <v>-288</v>
+      </c>
+      <c r="AP5" s="5">
+        <v>-299</v>
+      </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>1</v>
       </c>
@@ -11185,8 +11404,14 @@
       <c r="AN6" s="5">
         <v>44</v>
       </c>
+      <c r="AO6" s="5">
+        <v>47</v>
+      </c>
+      <c r="AP6" s="5">
+        <v>35</v>
+      </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>17</v>
       </c>
@@ -11301,8 +11526,14 @@
       <c r="AN7" s="5">
         <v>3622</v>
       </c>
+      <c r="AO7" s="5">
+        <v>2885</v>
+      </c>
+      <c r="AP7" s="5">
+        <v>2623</v>
+      </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -11312,7 +11543,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
@@ -11433,8 +11664,14 @@
       <c r="AN9" s="4" t="s">
         <v>50</v>
       </c>
+      <c r="AO9" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AP9" s="4" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>27</v>
       </c>
@@ -11555,8 +11792,14 @@
       <c r="AN10" s="5">
         <v>2308</v>
       </c>
+      <c r="AO10" s="5">
+        <v>1418</v>
+      </c>
+      <c r="AP10" s="5">
+        <v>851</v>
+      </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>0</v>
       </c>
@@ -11677,8 +11920,14 @@
       <c r="AN11" s="5">
         <v>39919</v>
       </c>
+      <c r="AO11" s="5">
+        <v>37414</v>
+      </c>
+      <c r="AP11" s="5">
+        <v>35329</v>
+      </c>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>15</v>
       </c>
@@ -11797,8 +12046,14 @@
       <c r="AN12" s="5">
         <v>7952</v>
       </c>
+      <c r="AO12" s="5">
+        <v>7664</v>
+      </c>
+      <c r="AP12" s="5">
+        <v>7365</v>
+      </c>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>1</v>
       </c>
@@ -11917,8 +12172,14 @@
       <c r="AN13" s="5">
         <v>2788</v>
       </c>
+      <c r="AO13" s="5">
+        <v>2835</v>
+      </c>
+      <c r="AP13" s="5">
+        <v>2870</v>
+      </c>
     </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>18</v>
       </c>
@@ -12032,6 +12293,12 @@
       </c>
       <c r="AN14" s="5">
         <v>36117</v>
+      </c>
+      <c r="AO14" s="5">
+        <v>39002</v>
+      </c>
+      <c r="AP14" s="5">
+        <v>41625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>